<commit_message>
Set max width of output columns to 50.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21516" windowHeight="7836"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21516" windowHeight="7836"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="241">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -333,9 +333,6 @@
     <t>Inv Date</t>
   </si>
   <si>
-    <t>Comm Type</t>
-  </si>
-  <si>
     <t>L1_Segm</t>
   </si>
   <si>
@@ -400,9 +397,6 @@
   </si>
   <si>
     <t>End Customer Market segment</t>
-  </si>
-  <si>
-    <t>Prod Country</t>
   </si>
   <si>
     <t>Material (Q-no.)</t>
@@ -719,6 +713,36 @@
   </si>
   <si>
     <t>CUSTOMER</t>
+  </si>
+  <si>
+    <t>CommissionDue</t>
+  </si>
+  <si>
+    <t>RecDate</t>
+  </si>
+  <si>
+    <t>CommissionPct</t>
+  </si>
+  <si>
+    <t>BillDocNo</t>
+  </si>
+  <si>
+    <t>GG</t>
+  </si>
+  <si>
+    <t>$ AMT</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Purchase Ord. No.</t>
+  </si>
+  <si>
+    <t>Extended Resale</t>
+  </si>
+  <si>
+    <t>Extended Cost</t>
   </si>
 </sst>
 </file>
@@ -1197,10 +1221,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF20"/>
+  <dimension ref="A1:AF21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14:L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1213,7 +1237,7 @@
     <col min="8" max="8" width="10.21875" customWidth="1"/>
     <col min="9" max="9" width="14.5546875" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="11" customWidth="1"/>
+    <col min="11" max="11" width="16.44140625" customWidth="1"/>
     <col min="12" max="12" width="16.21875" customWidth="1"/>
     <col min="13" max="13" width="17.44140625" customWidth="1"/>
     <col min="14" max="14" width="16.44140625" customWidth="1"/>
@@ -1249,10 +1273,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -1267,7 +1291,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
@@ -1347,10 +1371,10 @@
         <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G2" t="s">
         <v>49</v>
@@ -1359,13 +1383,13 @@
         <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J2" t="s">
         <v>61</v>
       </c>
       <c r="K2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="L2" t="s">
         <v>68</v>
@@ -1386,10 +1410,10 @@
         <v>97</v>
       </c>
       <c r="R2" t="s">
+        <v>237</v>
+      </c>
+      <c r="S2" t="s">
         <v>104</v>
-      </c>
-      <c r="S2" t="s">
-        <v>105</v>
       </c>
       <c r="T2" t="s">
         <v>15</v>
@@ -1398,37 +1422,37 @@
         <v>16</v>
       </c>
       <c r="V2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="W2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="X2" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y2" t="s">
         <v>118</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>119</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>120</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>121</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>122</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>123</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>124</v>
       </c>
-      <c r="AE2" t="s">
-        <v>125</v>
-      </c>
       <c r="AF2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
@@ -1445,10 +1469,10 @@
         <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G3" t="s">
         <v>50</v>
@@ -1463,7 +1487,7 @@
         <v>62</v>
       </c>
       <c r="K3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L3" t="s">
         <v>69</v>
@@ -1478,43 +1502,43 @@
         <v>86</v>
       </c>
       <c r="P3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="Q3" t="s">
         <v>98</v>
       </c>
       <c r="R3" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="S3" t="s">
         <v>14</v>
       </c>
       <c r="T3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="V3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="W3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="Y3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="AB3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="AC3" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="AE3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AF3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
@@ -1531,10 +1555,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F4" t="s">
         <v>223</v>
-      </c>
-      <c r="F4" t="s">
-        <v>225</v>
       </c>
       <c r="G4" t="s">
         <v>51</v>
@@ -1543,13 +1567,13 @@
         <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J4" t="s">
         <v>63</v>
       </c>
       <c r="K4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="L4" t="s">
         <v>70</v>
@@ -1570,28 +1594,25 @@
         <v>99</v>
       </c>
       <c r="S4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="U4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V4" t="s">
         <v>17</v>
       </c>
       <c r="W4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="Y4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="AE4" t="s">
         <v>26</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
@@ -1602,11 +1623,14 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
       </c>
+      <c r="E5" t="s">
+        <v>238</v>
+      </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
@@ -1614,11 +1638,14 @@
         <v>58</v>
       </c>
       <c r="I5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J5" t="s">
         <v>64</v>
       </c>
+      <c r="K5" t="s">
+        <v>240</v>
+      </c>
       <c r="L5" t="s">
         <v>71</v>
       </c>
@@ -1637,14 +1664,17 @@
       <c r="Q5" t="s">
         <v>12</v>
       </c>
+      <c r="S5" t="s">
+        <v>235</v>
+      </c>
       <c r="T5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="V5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="W5" t="s">
         <v>18</v>
@@ -1658,7 +1688,7 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -1679,7 +1709,7 @@
         <v>77</v>
       </c>
       <c r="N6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O6" t="s">
         <v>88</v>
@@ -1691,13 +1721,13 @@
         <v>100</v>
       </c>
       <c r="U6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="V6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="W6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
@@ -1708,10 +1738,10 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
@@ -1723,16 +1753,16 @@
         <v>66</v>
       </c>
       <c r="L7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="M7" t="s">
         <v>78</v>
       </c>
       <c r="N7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="O7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="P7" t="s">
         <v>94</v>
@@ -1741,13 +1771,13 @@
         <v>101</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="V7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="W7" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.3">
@@ -1755,10 +1785,10 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D8" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
@@ -1770,16 +1800,16 @@
         <v>6</v>
       </c>
       <c r="L8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="M8" t="s">
         <v>79</v>
       </c>
       <c r="N8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="O8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="P8" t="s">
         <v>95</v>
@@ -1788,10 +1818,10 @@
         <v>102</v>
       </c>
       <c r="U8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="V8" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
@@ -1799,28 +1829,28 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="J9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="L9" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="M9" t="s">
         <v>80</v>
       </c>
       <c r="O9" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="P9" t="s">
         <v>90</v>
@@ -1829,10 +1859,10 @@
         <v>103</v>
       </c>
       <c r="U9" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="V9" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
@@ -1840,191 +1870,211 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G10" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="L10" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="M10" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+      <c r="O10" t="s">
+        <v>233</v>
       </c>
       <c r="P10" t="s">
         <v>96</v>
       </c>
       <c r="Q10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D11" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G11" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="J11" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="M11" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="P11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="Q11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D12" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="G12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J12" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="L12" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="P12" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="Q12" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>158</v>
+        <v>156</v>
+      </c>
+      <c r="D13" t="s">
+        <v>234</v>
       </c>
       <c r="G13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="J13" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="L13" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="P13" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="Q13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L14" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="P14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="Q14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="L15" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="P15" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Q15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="G16" t="s">
-        <v>200</v>
+        <v>198</v>
+      </c>
+      <c r="L16" t="s">
+        <v>236</v>
       </c>
       <c r="P16" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="Q16" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G17" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
+      <c r="L17" t="s">
+        <v>239</v>
+      </c>
       <c r="P17" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="Q17" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="G18" t="s">
-        <v>217</v>
+        <v>215</v>
+      </c>
+      <c r="P18" t="s">
+        <v>231</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="G19" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="Q19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q20" t="s">
-        <v>227</v>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q21" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged Rep 1 % and Rep 2 % in OSR preprocessing.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="244">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -331,6 +331,9 @@
   </si>
   <si>
     <t>Inv Date</t>
+  </si>
+  <si>
+    <t>Comm Type</t>
   </si>
   <si>
     <t>L1_Segm</t>
@@ -743,6 +746,12 @@
   </si>
   <si>
     <t>Extended Cost</t>
+  </si>
+  <si>
+    <t>Name 11</t>
+  </si>
+  <si>
+    <t>INF Comm Type</t>
   </si>
 </sst>
 </file>
@@ -894,9 +903,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:AF25" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:AF25"/>
-  <tableColumns count="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:AG25" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:AG25"/>
+  <tableColumns count="33">
     <tableColumn id="1" name="Reported Customer"/>
     <tableColumn id="2" name="Reported End Customer"/>
     <tableColumn id="3" name="Distributor"/>
@@ -915,6 +924,7 @@
     <tableColumn id="12" name="Actual Comm Paid"/>
     <tableColumn id="13" name="Invoice Date"/>
     <tableColumn id="14" name="On/Offshore"/>
+    <tableColumn id="33" name="INF Comm Type"/>
     <tableColumn id="15" name="PL"/>
     <tableColumn id="16" name="Division"/>
     <tableColumn id="17" name="City"/>
@@ -1221,10 +1231,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF21"/>
+  <dimension ref="A1:AG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14:L15"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1244,22 +1254,22 @@
     <col min="15" max="15" width="17.33203125" customWidth="1"/>
     <col min="16" max="16" width="18.33203125" customWidth="1"/>
     <col min="17" max="17" width="13.33203125" customWidth="1"/>
-    <col min="18" max="18" width="13.5546875" customWidth="1"/>
-    <col min="20" max="20" width="9.44140625" customWidth="1"/>
-    <col min="21" max="21" width="18.77734375" customWidth="1"/>
-    <col min="23" max="23" width="10.21875" customWidth="1"/>
-    <col min="24" max="24" width="24.77734375" customWidth="1"/>
-    <col min="25" max="25" width="17.5546875" customWidth="1"/>
-    <col min="26" max="26" width="23.88671875" customWidth="1"/>
-    <col min="27" max="27" width="18" customWidth="1"/>
-    <col min="28" max="28" width="17" customWidth="1"/>
-    <col min="29" max="29" width="24.6640625" customWidth="1"/>
-    <col min="30" max="30" width="17.77734375" customWidth="1"/>
-    <col min="31" max="31" width="16.6640625" customWidth="1"/>
-    <col min="32" max="32" width="11.5546875" customWidth="1"/>
+    <col min="18" max="19" width="13.5546875" customWidth="1"/>
+    <col min="21" max="21" width="9.44140625" customWidth="1"/>
+    <col min="22" max="22" width="18.77734375" customWidth="1"/>
+    <col min="24" max="24" width="10.21875" customWidth="1"/>
+    <col min="25" max="25" width="24.77734375" customWidth="1"/>
+    <col min="26" max="26" width="17.5546875" customWidth="1"/>
+    <col min="27" max="27" width="23.88671875" customWidth="1"/>
+    <col min="28" max="28" width="18" customWidth="1"/>
+    <col min="29" max="29" width="17" customWidth="1"/>
+    <col min="30" max="30" width="24.6640625" customWidth="1"/>
+    <col min="31" max="31" width="17.77734375" customWidth="1"/>
+    <col min="32" max="32" width="16.6640625" customWidth="1"/>
+    <col min="33" max="33" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1273,10 +1283,10 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -1291,7 +1301,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
@@ -1315,49 +1325,52 @@
         <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1371,10 +1384,10 @@
         <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G2" t="s">
         <v>49</v>
@@ -1383,13 +1396,13 @@
         <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="J2" t="s">
         <v>61</v>
       </c>
       <c r="K2" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="L2" t="s">
         <v>68</v>
@@ -1410,25 +1423,25 @@
         <v>97</v>
       </c>
       <c r="R2" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="S2" t="s">
         <v>104</v>
       </c>
       <c r="T2" t="s">
+        <v>105</v>
+      </c>
+      <c r="U2" t="s">
         <v>15</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>16</v>
       </c>
-      <c r="V2" t="s">
-        <v>112</v>
-      </c>
       <c r="W2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="X2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="Y2" t="s">
         <v>118</v>
@@ -1452,10 +1465,13 @@
         <v>124</v>
       </c>
       <c r="AF2" t="s">
-        <v>126</v>
+        <v>125</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1469,10 +1485,10 @@
         <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G3" t="s">
         <v>50</v>
@@ -1487,7 +1503,7 @@
         <v>62</v>
       </c>
       <c r="K3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L3" t="s">
         <v>69</v>
@@ -1502,46 +1518,46 @@
         <v>86</v>
       </c>
       <c r="P3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="Q3" t="s">
         <v>98</v>
       </c>
       <c r="R3" t="s">
-        <v>210</v>
-      </c>
-      <c r="S3" t="s">
+        <v>211</v>
+      </c>
+      <c r="T3" t="s">
         <v>14</v>
       </c>
-      <c r="T3" t="s">
-        <v>105</v>
-      </c>
       <c r="U3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="V3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="W3" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>193</v>
-      </c>
-      <c r="AB3" t="s">
+        <v>114</v>
+      </c>
+      <c r="X3" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>194</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>206</v>
+      </c>
+      <c r="AD3" t="s">
         <v>205</v>
       </c>
-      <c r="AC3" t="s">
-        <v>204</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>125</v>
-      </c>
       <c r="AF3" t="s">
-        <v>127</v>
+        <v>126</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1555,10 +1571,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G4" t="s">
         <v>51</v>
@@ -1567,13 +1583,13 @@
         <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J4" t="s">
         <v>63</v>
       </c>
       <c r="K4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="L4" t="s">
         <v>70</v>
@@ -1593,29 +1609,29 @@
       <c r="Q4" t="s">
         <v>99</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
+        <v>108</v>
+      </c>
+      <c r="U4" t="s">
         <v>107</v>
       </c>
-      <c r="T4" t="s">
-        <v>106</v>
-      </c>
-      <c r="U4" t="s">
-        <v>109</v>
-      </c>
       <c r="V4" t="s">
+        <v>110</v>
+      </c>
+      <c r="W4" t="s">
         <v>17</v>
       </c>
-      <c r="W4" t="s">
-        <v>116</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>229</v>
-      </c>
-      <c r="AE4" t="s">
+      <c r="X4" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>230</v>
+      </c>
+      <c r="AF4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1623,13 +1639,13 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
@@ -1638,13 +1654,13 @@
         <v>58</v>
       </c>
       <c r="I5" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J5" t="s">
         <v>64</v>
       </c>
       <c r="K5" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="L5" t="s">
         <v>71</v>
@@ -1664,23 +1680,23 @@
       <c r="Q5" t="s">
         <v>12</v>
       </c>
-      <c r="S5" t="s">
-        <v>235</v>
-      </c>
       <c r="T5" t="s">
-        <v>107</v>
+        <v>236</v>
       </c>
       <c r="U5" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="V5" t="s">
-        <v>167</v>
+        <v>111</v>
       </c>
       <c r="W5" t="s">
+        <v>168</v>
+      </c>
+      <c r="X5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1688,7 +1704,7 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -1709,7 +1725,7 @@
         <v>77</v>
       </c>
       <c r="N6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="O6" t="s">
         <v>88</v>
@@ -1720,17 +1736,17 @@
       <c r="Q6" t="s">
         <v>100</v>
       </c>
-      <c r="U6" t="s">
-        <v>111</v>
-      </c>
       <c r="V6" t="s">
-        <v>186</v>
+        <v>112</v>
       </c>
       <c r="W6" t="s">
         <v>187</v>
       </c>
+      <c r="X6" t="s">
+        <v>188</v>
+      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1738,10 +1754,10 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D7" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
@@ -1753,16 +1769,16 @@
         <v>66</v>
       </c>
       <c r="L7" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M7" t="s">
         <v>78</v>
       </c>
       <c r="N7" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="O7" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="P7" t="s">
         <v>94</v>
@@ -1770,25 +1786,25 @@
       <c r="Q7" t="s">
         <v>101</v>
       </c>
-      <c r="U7" s="2" t="s">
-        <v>159</v>
-      </c>
-      <c r="V7" t="s">
-        <v>188</v>
+      <c r="V7" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="W7" t="s">
-        <v>222</v>
+        <v>189</v>
+      </c>
+      <c r="X7" t="s">
+        <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
@@ -1800,16 +1816,16 @@
         <v>6</v>
       </c>
       <c r="L8" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="M8" t="s">
         <v>79</v>
       </c>
       <c r="N8" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="O8" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="P8" t="s">
         <v>95</v>
@@ -1817,40 +1833,40 @@
       <c r="Q8" t="s">
         <v>102</v>
       </c>
-      <c r="U8" t="s">
-        <v>185</v>
-      </c>
       <c r="V8" t="s">
-        <v>203</v>
+        <v>186</v>
+      </c>
+      <c r="W8" t="s">
+        <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D9" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G9" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H9" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="J9" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L9" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="M9" t="s">
         <v>80</v>
       </c>
       <c r="O9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="P9" t="s">
         <v>90</v>
@@ -1858,223 +1874,226 @@
       <c r="Q9" t="s">
         <v>103</v>
       </c>
-      <c r="U9" t="s">
-        <v>202</v>
-      </c>
       <c r="V9" t="s">
-        <v>224</v>
+        <v>203</v>
+      </c>
+      <c r="W9" t="s">
+        <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H10" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="J10" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="L10" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="M10" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="O10" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P10" t="s">
         <v>96</v>
       </c>
       <c r="Q10" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="D11" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G11" t="s">
+        <v>140</v>
+      </c>
+      <c r="J11" t="s">
+        <v>177</v>
+      </c>
+      <c r="L11" t="s">
+        <v>176</v>
+      </c>
+      <c r="M11" t="s">
+        <v>167</v>
+      </c>
+      <c r="P11" t="s">
+        <v>141</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" t="s">
+        <v>228</v>
+      </c>
+      <c r="G12" t="s">
+        <v>156</v>
+      </c>
+      <c r="J12" t="s">
+        <v>180</v>
+      </c>
+      <c r="L12" t="s">
+        <v>178</v>
+      </c>
+      <c r="M12" t="s">
+        <v>201</v>
+      </c>
+      <c r="P12" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q12" t="s">
         <v>139</v>
       </c>
-      <c r="J11" t="s">
-        <v>176</v>
-      </c>
-      <c r="L11" t="s">
-        <v>175</v>
-      </c>
-      <c r="M11" t="s">
-        <v>166</v>
-      </c>
-      <c r="P11" t="s">
-        <v>140</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>136</v>
-      </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D12" t="s">
-        <v>227</v>
-      </c>
-      <c r="G12" t="s">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" t="s">
+        <v>235</v>
+      </c>
+      <c r="G13" t="s">
+        <v>158</v>
+      </c>
+      <c r="J13" t="s">
+        <v>215</v>
+      </c>
+      <c r="L13" t="s">
+        <v>181</v>
+      </c>
+      <c r="P13" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q13" t="s">
         <v>155</v>
       </c>
-      <c r="J12" t="s">
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>174</v>
+      </c>
+      <c r="G14" t="s">
+        <v>171</v>
+      </c>
+      <c r="L14" t="s">
+        <v>193</v>
+      </c>
+      <c r="P14" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q14" t="s">
         <v>179</v>
       </c>
-      <c r="L12" t="s">
-        <v>177</v>
-      </c>
-      <c r="M12" t="s">
-        <v>200</v>
-      </c>
-      <c r="P12" t="s">
-        <v>143</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>138</v>
-      </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>156</v>
-      </c>
-      <c r="D13" t="s">
-        <v>234</v>
-      </c>
-      <c r="G13" t="s">
-        <v>157</v>
-      </c>
-      <c r="J13" t="s">
-        <v>214</v>
-      </c>
-      <c r="L13" t="s">
-        <v>180</v>
-      </c>
-      <c r="P13" t="s">
-        <v>142</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>154</v>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>184</v>
+      </c>
+      <c r="G15" t="s">
+        <v>191</v>
+      </c>
+      <c r="L15" t="s">
+        <v>229</v>
+      </c>
+      <c r="P15" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>173</v>
-      </c>
-      <c r="G14" t="s">
-        <v>170</v>
-      </c>
-      <c r="L14" t="s">
-        <v>192</v>
-      </c>
-      <c r="P14" t="s">
-        <v>160</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>183</v>
-      </c>
-      <c r="G15" t="s">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>198</v>
+      </c>
+      <c r="G16" t="s">
+        <v>199</v>
+      </c>
+      <c r="L16" t="s">
+        <v>237</v>
+      </c>
+      <c r="P16" t="s">
+        <v>182</v>
+      </c>
+      <c r="Q16" t="s">
         <v>190</v>
-      </c>
-      <c r="L15" t="s">
-        <v>228</v>
-      </c>
-      <c r="P15" t="s">
-        <v>171</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>197</v>
-      </c>
-      <c r="G16" t="s">
-        <v>198</v>
-      </c>
-      <c r="L16" t="s">
-        <v>236</v>
-      </c>
-      <c r="P16" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G17" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="P17" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q17" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="G18" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="P18" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="Q18" s="4" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>242</v>
+      </c>
       <c r="G19" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="Q19" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="Q21" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the ATS special processing for new format.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="245">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -752,6 +752,9 @@
   </si>
   <si>
     <t>INF Comm Type</t>
+  </si>
+  <si>
+    <t>ComRate</t>
   </si>
 </sst>
 </file>
@@ -1233,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1935,6 +1938,9 @@
       <c r="M11" t="s">
         <v>167</v>
       </c>
+      <c r="O11" t="s">
+        <v>244</v>
+      </c>
       <c r="P11" t="s">
         <v>141</v>
       </c>

</xml_diff>

<commit_message>
Fxied Osram mapping for Invoice Date on POS tab.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="246">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -755,6 +755,9 @@
   </si>
   <si>
     <t>ComRate</t>
+  </si>
+  <si>
+    <t>POS Invoice Date</t>
   </si>
 </sst>
 </file>
@@ -1234,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG21"/>
+  <dimension ref="A1:AG22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1256,7 +1259,7 @@
     <col min="14" max="14" width="16.44140625" customWidth="1"/>
     <col min="15" max="15" width="17.33203125" customWidth="1"/>
     <col min="16" max="16" width="18.33203125" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" customWidth="1"/>
+    <col min="17" max="17" width="14.33203125" customWidth="1"/>
     <col min="18" max="19" width="13.5546875" customWidth="1"/>
     <col min="21" max="21" width="9.44140625" customWidth="1"/>
     <col min="22" max="22" width="18.77734375" customWidth="1"/>
@@ -2102,6 +2105,11 @@
         <v>233</v>
       </c>
     </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q22" t="s">
+        <v>245</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Changed Distributor column to Reported Distributor.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="247">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -758,6 +758,9 @@
   </si>
   <si>
     <t>POS Invoice Date</t>
+  </si>
+  <si>
+    <t>Reported Distributor</t>
   </si>
 </sst>
 </file>
@@ -914,7 +917,7 @@
   <tableColumns count="33">
     <tableColumn id="1" name="Reported Customer"/>
     <tableColumn id="2" name="Reported End Customer"/>
-    <tableColumn id="3" name="Distributor"/>
+    <tableColumn id="3" name="Reported Distributor"/>
     <tableColumn id="4" name="Invoice Number"/>
     <tableColumn id="30" name="PO Number"/>
     <tableColumn id="29" name="Sales Order #"/>
@@ -1239,8 +1242,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1283,7 +1286,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>246</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Updated part number mapping for QRF.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="248">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -761,6 +761,9 @@
   </si>
   <si>
     <t>Reported Distributor</t>
+  </si>
+  <si>
+    <t>Material</t>
   </si>
 </sst>
 </file>
@@ -1242,8 +1245,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AG22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2099,6 +2102,9 @@
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>247</v>
+      </c>
       <c r="Q20" t="s">
         <v>226</v>
       </c>

</xml_diff>

<commit_message>
Fixed default datetime formats.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21516" windowHeight="7836"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21516" windowHeight="7836"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup" sheetId="1" r:id="rId1"/>
@@ -1264,7 +1264,7 @@
   <dimension ref="A1:AG22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Setting directory path when GUI launches.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21516" windowHeight="7836"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21516" windowHeight="7836"/>
   </bookViews>
   <sheets>
     <sheet name="Lookup" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="255">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -782,6 +782,9 @@
   </si>
   <si>
     <t>Comm.  Amt</t>
+  </si>
+  <si>
+    <t>ShipDate</t>
   </si>
 </sst>
 </file>
@@ -1261,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG22"/>
+  <dimension ref="A1:AG23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2155,6 +2158,11 @@
         <v>245</v>
       </c>
     </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q23" t="s">
+        <v>254</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Switched use case of WriteComments for Digikey program.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="257">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -785,6 +785,12 @@
   </si>
   <si>
     <t>ShipDate</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Comm Source</t>
   </si>
 </sst>
 </file>
@@ -936,9 +942,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:AG25" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:AG25"/>
-  <tableColumns count="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:AI25" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
+  <autoFilter ref="A1:AI25"/>
+  <tableColumns count="35">
     <tableColumn id="1" name="Reported Customer"/>
     <tableColumn id="2" name="Reported End Customer"/>
     <tableColumn id="3" name="Reported Distributor"/>
@@ -955,6 +961,7 @@
     <tableColumn id="10" name="Split Percentage"/>
     <tableColumn id="11" name="Commission Rate"/>
     <tableColumn id="12" name="Actual Comm Paid"/>
+    <tableColumn id="35" name="Comm Source"/>
     <tableColumn id="13" name="Invoice Date"/>
     <tableColumn id="14" name="On/Offshore"/>
     <tableColumn id="33" name="INF Comm Type"/>
@@ -964,6 +971,7 @@
     <tableColumn id="18" name="State"/>
     <tableColumn id="19" name="Zip Code"/>
     <tableColumn id="20" name="Gross Rev Reduction"/>
+    <tableColumn id="34" name="Project"/>
     <tableColumn id="21" name="Product Category"/>
     <tableColumn id="22" name="Shared Rev Tier Rate"/>
     <tableColumn id="23" name="Cust Revenue YTD"/>
@@ -1264,10 +1272,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG23"/>
+  <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1285,24 +1293,25 @@
     <col min="13" max="13" width="17.44140625" customWidth="1"/>
     <col min="14" max="14" width="16.44140625" customWidth="1"/>
     <col min="15" max="15" width="17.33203125" customWidth="1"/>
-    <col min="16" max="16" width="18.33203125" customWidth="1"/>
-    <col min="17" max="17" width="14.33203125" customWidth="1"/>
-    <col min="18" max="19" width="13.5546875" customWidth="1"/>
-    <col min="21" max="21" width="9.44140625" customWidth="1"/>
-    <col min="22" max="22" width="18.77734375" customWidth="1"/>
-    <col min="24" max="24" width="10.21875" customWidth="1"/>
-    <col min="25" max="25" width="24.77734375" customWidth="1"/>
-    <col min="26" max="26" width="17.5546875" customWidth="1"/>
-    <col min="27" max="27" width="23.88671875" customWidth="1"/>
-    <col min="28" max="28" width="18" customWidth="1"/>
-    <col min="29" max="29" width="17" customWidth="1"/>
-    <col min="30" max="30" width="24.6640625" customWidth="1"/>
-    <col min="31" max="31" width="17.77734375" customWidth="1"/>
-    <col min="32" max="32" width="16.6640625" customWidth="1"/>
-    <col min="33" max="33" width="11.5546875" customWidth="1"/>
+    <col min="16" max="17" width="18.33203125" customWidth="1"/>
+    <col min="18" max="18" width="14.33203125" customWidth="1"/>
+    <col min="19" max="20" width="13.5546875" customWidth="1"/>
+    <col min="22" max="22" width="9.44140625" customWidth="1"/>
+    <col min="23" max="23" width="18.77734375" customWidth="1"/>
+    <col min="25" max="25" width="10.21875" customWidth="1"/>
+    <col min="26" max="26" width="24.77734375" customWidth="1"/>
+    <col min="27" max="27" width="16.6640625" customWidth="1"/>
+    <col min="28" max="28" width="17.5546875" customWidth="1"/>
+    <col min="29" max="29" width="23.88671875" customWidth="1"/>
+    <col min="30" max="30" width="18" customWidth="1"/>
+    <col min="31" max="31" width="17" customWidth="1"/>
+    <col min="32" max="32" width="24.6640625" customWidth="1"/>
+    <col min="33" max="33" width="17.77734375" customWidth="1"/>
+    <col min="34" max="34" width="16.6640625" customWidth="1"/>
+    <col min="35" max="35" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1352,58 +1361,64 @@
         <v>11</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="AB1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>28</v>
       </c>
@@ -1453,58 +1468,64 @@
         <v>89</v>
       </c>
       <c r="Q2" t="s">
+        <v>256</v>
+      </c>
+      <c r="R2" t="s">
         <v>97</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>238</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>104</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>105</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>15</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>16</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>113</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>115</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>118</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
+        <v>255</v>
+      </c>
+      <c r="AB2" t="s">
         <v>119</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>120</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>121</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>122</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AF2" t="s">
         <v>123</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AG2" t="s">
         <v>124</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AH2" t="s">
         <v>125</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AI2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1553,44 +1574,44 @@
       <c r="P3" t="s">
         <v>153</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>98</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>211</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>14</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>106</v>
       </c>
-      <c r="V3" t="s">
+      <c r="W3" t="s">
         <v>109</v>
       </c>
-      <c r="W3" t="s">
+      <c r="X3" t="s">
         <v>114</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>116</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>194</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AE3" t="s">
         <v>206</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AF3" t="s">
         <v>205</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AH3" t="s">
         <v>126</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AI3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -1639,32 +1660,32 @@
       <c r="P4" t="s">
         <v>91</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>99</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>108</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>107</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>110</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>17</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>117</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AB4" t="s">
         <v>230</v>
       </c>
-      <c r="AF4" t="s">
+      <c r="AH4" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1710,26 +1731,26 @@
       <c r="P5" t="s">
         <v>92</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>12</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>236</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>108</v>
       </c>
-      <c r="V5" t="s">
+      <c r="W5" t="s">
         <v>111</v>
       </c>
-      <c r="W5" t="s">
+      <c r="X5" t="s">
         <v>168</v>
       </c>
-      <c r="X5" t="s">
+      <c r="Y5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1766,20 +1787,20 @@
       <c r="P6" t="s">
         <v>93</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>100</v>
       </c>
-      <c r="V6" t="s">
+      <c r="W6" t="s">
         <v>112</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>187</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -1816,20 +1837,20 @@
       <c r="P7" t="s">
         <v>94</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>101</v>
       </c>
-      <c r="V7" s="2" t="s">
+      <c r="W7" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>189</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1863,17 +1884,17 @@
       <c r="P8" t="s">
         <v>95</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>102</v>
       </c>
-      <c r="V8" t="s">
+      <c r="W8" t="s">
         <v>186</v>
       </c>
-      <c r="W8" t="s">
+      <c r="X8" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -1904,17 +1925,17 @@
       <c r="P9" t="s">
         <v>90</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>103</v>
       </c>
-      <c r="V9" t="s">
+      <c r="W9" t="s">
         <v>203</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1945,11 +1966,11 @@
       <c r="P10" t="s">
         <v>96</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>131</v>
       </c>
@@ -1977,11 +1998,11 @@
       <c r="P11" t="s">
         <v>141</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>151</v>
       </c>
@@ -2003,11 +2024,11 @@
       <c r="P12" t="s">
         <v>144</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>157</v>
       </c>
@@ -2026,11 +2047,11 @@
       <c r="P13" t="s">
         <v>143</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>174</v>
       </c>
@@ -2043,11 +2064,11 @@
       <c r="P14" t="s">
         <v>161</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>184</v>
       </c>
@@ -2060,11 +2081,11 @@
       <c r="P15" t="s">
         <v>172</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>198</v>
       </c>
@@ -2077,11 +2098,11 @@
       <c r="P16" t="s">
         <v>182</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>219</v>
       </c>
@@ -2096,11 +2117,11 @@
       <c r="P17" t="s">
         <v>209</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>231</v>
       </c>
@@ -2113,11 +2134,11 @@
       <c r="P18" t="s">
         <v>232</v>
       </c>
-      <c r="Q18" s="4" t="s">
+      <c r="R18" s="4" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>242</v>
       </c>
@@ -2127,11 +2148,11 @@
       <c r="P19" t="s">
         <v>249</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>251</v>
       </c>
@@ -2141,25 +2162,25 @@
       <c r="P20" t="s">
         <v>253</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G21" t="s">
         <v>248</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="Q22" t="s">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R22" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="Q23" t="s">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="R23" t="s">
         <v>254</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Working on salesperson reports code.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="256">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -262,9 +262,6 @@
   </si>
   <si>
     <t>Value</t>
-  </si>
-  <si>
-    <t>Comm %</t>
   </si>
   <si>
     <t>Comm.%</t>
@@ -1274,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1319,16 +1316,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -1343,7 +1340,7 @@
         <v>6</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>7</v>
@@ -1361,7 +1358,7 @@
         <v>11</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>12</v>
@@ -1370,7 +1367,7 @@
         <v>13</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>14</v>
@@ -1391,7 +1388,7 @@
         <v>19</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="AB1" s="1" t="s">
         <v>20</v>
@@ -1432,10 +1429,10 @@
         <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G2" t="s">
         <v>49</v>
@@ -1444,13 +1441,13 @@
         <v>55</v>
       </c>
       <c r="I2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="J2" t="s">
         <v>61</v>
       </c>
       <c r="K2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="L2" t="s">
         <v>68</v>
@@ -1459,28 +1456,28 @@
         <v>73</v>
       </c>
       <c r="N2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="P2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="Q2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="R2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="T2" t="s">
+        <v>103</v>
+      </c>
+      <c r="U2" t="s">
         <v>104</v>
-      </c>
-      <c r="U2" t="s">
-        <v>105</v>
       </c>
       <c r="V2" t="s">
         <v>15</v>
@@ -1489,40 +1486,40 @@
         <v>16</v>
       </c>
       <c r="X2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Z2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>254</v>
+      </c>
+      <c r="AB2" t="s">
         <v>118</v>
       </c>
-      <c r="AA2" t="s">
-        <v>255</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>119</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>120</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>121</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>122</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>123</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>124</v>
       </c>
-      <c r="AH2" t="s">
-        <v>125</v>
-      </c>
       <c r="AI2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.3">
@@ -1539,10 +1536,10 @@
         <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G3" t="s">
         <v>50</v>
@@ -1557,7 +1554,7 @@
         <v>62</v>
       </c>
       <c r="K3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L3" t="s">
         <v>69</v>
@@ -1566,49 +1563,49 @@
         <v>74</v>
       </c>
       <c r="N3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="P3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="U3" t="s">
         <v>14</v>
       </c>
       <c r="V3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="W3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="Y3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AB3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AE3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AF3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="AH3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AI3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.3">
@@ -1625,10 +1622,10 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G4" t="s">
         <v>51</v>
@@ -1637,13 +1634,13 @@
         <v>57</v>
       </c>
       <c r="I4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J4" t="s">
         <v>63</v>
       </c>
       <c r="K4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="L4" t="s">
         <v>70</v>
@@ -1652,34 +1649,34 @@
         <v>75</v>
       </c>
       <c r="N4" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="O4" t="s">
         <v>10</v>
       </c>
       <c r="P4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="R4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="U4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="V4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="W4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="X4" t="s">
         <v>17</v>
       </c>
       <c r="Y4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AB4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AH4" t="s">
         <v>26</v>
@@ -1693,13 +1690,13 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D5" t="s">
         <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G5" t="s">
         <v>4</v>
@@ -1708,13 +1705,13 @@
         <v>58</v>
       </c>
       <c r="I5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J5" t="s">
         <v>64</v>
       </c>
       <c r="K5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="L5" t="s">
         <v>71</v>
@@ -1723,28 +1720,28 @@
         <v>76</v>
       </c>
       <c r="N5" t="s">
-        <v>84</v>
+        <v>207</v>
       </c>
       <c r="O5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="P5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="R5" t="s">
         <v>12</v>
       </c>
       <c r="U5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="V5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="W5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="X5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="Y5" t="s">
         <v>18</v>
@@ -1758,7 +1755,7 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -1778,26 +1775,23 @@
       <c r="M6" t="s">
         <v>77</v>
       </c>
-      <c r="N6" t="s">
-        <v>135</v>
-      </c>
       <c r="O6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="P6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="R6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="W6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="X6" t="s">
+        <v>186</v>
+      </c>
+      <c r="Y6" t="s">
         <v>187</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.3">
@@ -1808,10 +1802,10 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
@@ -1823,31 +1817,28 @@
         <v>66</v>
       </c>
       <c r="L7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M7" t="s">
         <v>78</v>
       </c>
-      <c r="N7" t="s">
-        <v>162</v>
-      </c>
       <c r="O7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="X7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="Y7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.3">
@@ -1855,10 +1846,10 @@
         <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G8" t="s">
         <v>54</v>
@@ -1870,28 +1861,25 @@
         <v>6</v>
       </c>
       <c r="L8" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M8" t="s">
         <v>79</v>
       </c>
-      <c r="N8" t="s">
-        <v>208</v>
-      </c>
       <c r="O8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P8" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="R8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="W8" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="X8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
@@ -1899,40 +1887,40 @@
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H9" t="s">
         <v>132</v>
       </c>
-      <c r="H9" t="s">
-        <v>133</v>
-      </c>
       <c r="J9" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="L9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="M9" t="s">
         <v>80</v>
       </c>
       <c r="O9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="P9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="W9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="X9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.3">
@@ -1940,248 +1928,254 @@
         <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H10" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="L10" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="M10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O10" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B11" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D11" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G11" t="s">
+        <v>139</v>
+      </c>
+      <c r="J11" t="s">
+        <v>176</v>
+      </c>
+      <c r="L11" t="s">
+        <v>175</v>
+      </c>
+      <c r="M11" t="s">
+        <v>166</v>
+      </c>
+      <c r="O11" t="s">
+        <v>243</v>
+      </c>
+      <c r="P11" t="s">
         <v>140</v>
       </c>
-      <c r="J11" t="s">
-        <v>177</v>
-      </c>
-      <c r="L11" t="s">
-        <v>176</v>
-      </c>
-      <c r="M11" t="s">
-        <v>167</v>
-      </c>
-      <c r="O11" t="s">
-        <v>244</v>
-      </c>
-      <c r="P11" t="s">
-        <v>141</v>
-      </c>
       <c r="R11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D12" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="G12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J12" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M12" t="s">
-        <v>201</v>
+        <v>200</v>
+      </c>
+      <c r="O12" t="s">
+        <v>161</v>
       </c>
       <c r="P12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="R12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" t="s">
+        <v>234</v>
+      </c>
+      <c r="G13" t="s">
         <v>157</v>
       </c>
-      <c r="D13" t="s">
-        <v>235</v>
-      </c>
-      <c r="G13" t="s">
-        <v>158</v>
-      </c>
       <c r="J13" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="L13" t="s">
-        <v>181</v>
+        <v>180</v>
+      </c>
+      <c r="O13" t="s">
+        <v>81</v>
       </c>
       <c r="P13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="R13" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G14" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="L14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="R14" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="G15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="L15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="P15" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="R15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>197</v>
+      </c>
+      <c r="G16" t="s">
         <v>198</v>
       </c>
-      <c r="G16" t="s">
-        <v>199</v>
-      </c>
       <c r="L16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P16" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="R16" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G17" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="R17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>230</v>
+      </c>
+      <c r="G18" t="s">
+        <v>215</v>
+      </c>
+      <c r="L18" t="s">
+        <v>249</v>
+      </c>
+      <c r="P18" t="s">
         <v>231</v>
       </c>
-      <c r="G18" t="s">
-        <v>216</v>
-      </c>
-      <c r="L18" t="s">
-        <v>250</v>
-      </c>
-      <c r="P18" t="s">
-        <v>232</v>
-      </c>
       <c r="R18" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="P19" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="R19" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="R21" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R22" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R23" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Sales reports now include principal and customer tables.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -1271,8 +1271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Removing table formatting from Excel outputs.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -15,11 +15,12 @@
     <sheet name="Lookup" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="265">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -791,6 +792,30 @@
   </si>
   <si>
     <t>Material (Q-no.) Name</t>
+  </si>
+  <si>
+    <t>End Customer value</t>
+  </si>
+  <si>
+    <t>Tota Comm</t>
+  </si>
+  <si>
+    <t>Postal Code</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Disti costs value</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>HS</t>
+  </si>
+  <si>
+    <t>KC</t>
   </si>
 </sst>
 </file>
@@ -1272,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI23"/>
+  <dimension ref="A1:AI2561"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1289,7 +1314,7 @@
     <col min="9" max="9" width="14.5546875" customWidth="1"/>
     <col min="10" max="10" width="18" customWidth="1"/>
     <col min="11" max="11" width="16.44140625" customWidth="1"/>
-    <col min="12" max="12" width="16.21875" customWidth="1"/>
+    <col min="12" max="12" width="19.5546875" customWidth="1"/>
     <col min="13" max="13" width="17.44140625" customWidth="1"/>
     <col min="14" max="14" width="16.44140625" customWidth="1"/>
     <col min="15" max="15" width="17.33203125" customWidth="1"/>
@@ -1772,6 +1797,9 @@
       <c r="J6" t="s">
         <v>65</v>
       </c>
+      <c r="K6" t="s">
+        <v>261</v>
+      </c>
       <c r="L6" t="s">
         <v>72</v>
       </c>
@@ -1884,6 +1912,9 @@
       <c r="X8" t="s">
         <v>203</v>
       </c>
+      <c r="Y8" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
@@ -1960,6 +1991,9 @@
       <c r="R10" t="s">
         <v>128</v>
       </c>
+      <c r="W10" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -2035,6 +2069,9 @@
       <c r="L13" t="s">
         <v>180</v>
       </c>
+      <c r="M13" t="s">
+        <v>257</v>
+      </c>
       <c r="O13" t="s">
         <v>81</v>
       </c>
@@ -2048,6 +2085,9 @@
     <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>173</v>
+      </c>
+      <c r="D14" t="s">
+        <v>262</v>
       </c>
       <c r="G14" t="s">
         <v>170</v>
@@ -2167,6 +2207,9 @@
       <c r="G21" t="s">
         <v>247</v>
       </c>
+      <c r="P21" t="s">
+        <v>258</v>
+      </c>
       <c r="R21" t="s">
         <v>232</v>
       </c>
@@ -2182,6 +2225,16 @@
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="R23" t="s">
         <v>253</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2350" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2561" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switched column order in Running Commissions.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -972,22 +972,22 @@
   <tableColumns count="35">
     <tableColumn id="1" name="Reported Customer"/>
     <tableColumn id="2" name="Reported End Customer"/>
-    <tableColumn id="3" name="Reported Distributor"/>
     <tableColumn id="4" name="Invoice Number"/>
-    <tableColumn id="30" name="PO Number"/>
-    <tableColumn id="29" name="Sales Order #"/>
     <tableColumn id="5" name="Part Number"/>
     <tableColumn id="6" name="Quantity"/>
-    <tableColumn id="31" name="Unit Cost"/>
-    <tableColumn id="7" name="Unit Price"/>
     <tableColumn id="32" name="Ext. Cost"/>
     <tableColumn id="8" name="Invoiced Dollars"/>
     <tableColumn id="9" name="Paid-On Revenue"/>
     <tableColumn id="10" name="Split Percentage"/>
     <tableColumn id="11" name="Commission Rate"/>
     <tableColumn id="12" name="Actual Comm Paid"/>
-    <tableColumn id="35" name="Comm Source"/>
     <tableColumn id="13" name="Invoice Date"/>
+    <tableColumn id="36" name="Reported Distributor"/>
+    <tableColumn id="37" name="PO Number"/>
+    <tableColumn id="38" name="Sales Order #"/>
+    <tableColumn id="40" name="Unit Cost"/>
+    <tableColumn id="39" name="Unit Price"/>
+    <tableColumn id="41" name="Comm Source"/>
     <tableColumn id="14" name="On/Offshore"/>
     <tableColumn id="33" name="INF Comm Type"/>
     <tableColumn id="15" name="PL"/>
@@ -1300,26 +1300,24 @@
   <dimension ref="A1:AI2561"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="R12" sqref="R12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="22.21875" customWidth="1"/>
     <col min="2" max="2" width="22.88671875" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
-    <col min="4" max="6" width="16.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="16.44140625" customWidth="1"/>
-    <col min="12" max="12" width="19.5546875" customWidth="1"/>
-    <col min="13" max="13" width="17.44140625" customWidth="1"/>
-    <col min="14" max="14" width="16.44140625" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" customWidth="1"/>
-    <col min="16" max="17" width="18.33203125" customWidth="1"/>
-    <col min="18" max="18" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="5" max="5" width="10.21875" customWidth="1"/>
+    <col min="6" max="6" width="16.44140625" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" customWidth="1"/>
+    <col min="8" max="8" width="17.44140625" customWidth="1"/>
+    <col min="9" max="9" width="16.44140625" customWidth="1"/>
+    <col min="10" max="10" width="17.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="18" width="26.6640625" customWidth="1"/>
     <col min="19" max="20" width="13.5546875" customWidth="1"/>
     <col min="22" max="22" width="9.44140625" customWidth="1"/>
     <col min="23" max="23" width="18.77734375" customWidth="1"/>
@@ -1344,52 +1342,52 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>255</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>13</v>
@@ -1451,52 +1449,52 @@
         <v>37</v>
       </c>
       <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" t="s">
+        <v>82</v>
+      </c>
+      <c r="J2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K2" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" t="s">
+        <v>96</v>
+      </c>
+      <c r="M2" t="s">
         <v>43</v>
       </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="N2" t="s">
         <v>164</v>
       </c>
-      <c r="F2" t="s">
+      <c r="O2" t="s">
         <v>147</v>
       </c>
-      <c r="G2" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="P2" t="s">
         <v>194</v>
       </c>
-      <c r="J2" t="s">
+      <c r="Q2" t="s">
         <v>61</v>
       </c>
-      <c r="K2" t="s">
-        <v>196</v>
-      </c>
-      <c r="L2" t="s">
-        <v>68</v>
-      </c>
-      <c r="M2" t="s">
-        <v>73</v>
-      </c>
-      <c r="N2" t="s">
-        <v>82</v>
-      </c>
-      <c r="O2" t="s">
-        <v>84</v>
-      </c>
-      <c r="P2" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>255</v>
-      </c>
-      <c r="R2" t="s">
-        <v>96</v>
       </c>
       <c r="S2" t="s">
         <v>237</v>
@@ -1558,49 +1556,49 @@
         <v>38</v>
       </c>
       <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" t="s">
+        <v>195</v>
+      </c>
+      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+      <c r="I3" t="s">
+        <v>83</v>
+      </c>
+      <c r="J3" t="s">
+        <v>85</v>
+      </c>
+      <c r="K3" t="s">
+        <v>152</v>
+      </c>
+      <c r="L3" t="s">
+        <v>97</v>
+      </c>
+      <c r="M3" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="N3" t="s">
         <v>163</v>
       </c>
-      <c r="F3" t="s">
+      <c r="O3" t="s">
         <v>213</v>
       </c>
-      <c r="G3" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I3" t="s">
+      <c r="P3" t="s">
         <v>67</v>
       </c>
-      <c r="J3" t="s">
+      <c r="Q3" t="s">
         <v>62</v>
-      </c>
-      <c r="K3" t="s">
-        <v>195</v>
-      </c>
-      <c r="L3" t="s">
-        <v>69</v>
-      </c>
-      <c r="M3" t="s">
-        <v>74</v>
-      </c>
-      <c r="N3" t="s">
-        <v>83</v>
-      </c>
-      <c r="O3" t="s">
-        <v>85</v>
-      </c>
-      <c r="P3" t="s">
-        <v>152</v>
-      </c>
-      <c r="R3" t="s">
-        <v>97</v>
       </c>
       <c r="S3" t="s">
         <v>210</v>
@@ -1644,49 +1642,49 @@
         <v>39</v>
       </c>
       <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" t="s">
+        <v>75</v>
+      </c>
+      <c r="I4" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" t="s">
+        <v>98</v>
+      </c>
+      <c r="M4" t="s">
         <v>44</v>
       </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="N4" t="s">
         <v>221</v>
       </c>
-      <c r="F4" t="s">
+      <c r="O4" t="s">
         <v>223</v>
       </c>
-      <c r="G4" t="s">
-        <v>51</v>
-      </c>
-      <c r="H4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="P4" t="s">
         <v>209</v>
       </c>
-      <c r="J4" t="s">
+      <c r="Q4" t="s">
         <v>63</v>
-      </c>
-      <c r="K4" t="s">
-        <v>217</v>
-      </c>
-      <c r="L4" t="s">
-        <v>70</v>
-      </c>
-      <c r="M4" t="s">
-        <v>75</v>
-      </c>
-      <c r="N4" t="s">
-        <v>134</v>
-      </c>
-      <c r="O4" t="s">
-        <v>10</v>
-      </c>
-      <c r="P4" t="s">
-        <v>90</v>
-      </c>
-      <c r="R4" t="s">
-        <v>98</v>
       </c>
       <c r="U4" t="s">
         <v>107</v>
@@ -1718,46 +1716,46 @@
         <v>40</v>
       </c>
       <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G5" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" t="s">
+        <v>76</v>
+      </c>
+      <c r="I5" t="s">
+        <v>207</v>
+      </c>
+      <c r="J5" t="s">
+        <v>86</v>
+      </c>
+      <c r="K5" t="s">
+        <v>91</v>
+      </c>
+      <c r="L5" t="s">
+        <v>12</v>
+      </c>
+      <c r="M5" t="s">
         <v>151</v>
       </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="N5" t="s">
         <v>238</v>
       </c>
-      <c r="G5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="P5" t="s">
         <v>216</v>
       </c>
-      <c r="J5" t="s">
+      <c r="Q5" t="s">
         <v>64</v>
-      </c>
-      <c r="K5" t="s">
-        <v>240</v>
-      </c>
-      <c r="L5" t="s">
-        <v>71</v>
-      </c>
-      <c r="M5" t="s">
-        <v>76</v>
-      </c>
-      <c r="N5" t="s">
-        <v>207</v>
-      </c>
-      <c r="O5" t="s">
-        <v>86</v>
-      </c>
-      <c r="P5" t="s">
-        <v>91</v>
-      </c>
-      <c r="R5" t="s">
-        <v>12</v>
       </c>
       <c r="U5" t="s">
         <v>235</v>
@@ -1783,37 +1781,37 @@
         <v>41</v>
       </c>
       <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" t="s">
+        <v>261</v>
+      </c>
+      <c r="G6" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" t="s">
+        <v>77</v>
+      </c>
+      <c r="J6" t="s">
+        <v>87</v>
+      </c>
+      <c r="K6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L6" t="s">
+        <v>99</v>
+      </c>
+      <c r="M6" t="s">
         <v>129</v>
       </c>
-      <c r="D6" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="Q6" t="s">
         <v>65</v>
-      </c>
-      <c r="K6" t="s">
-        <v>261</v>
-      </c>
-      <c r="L6" t="s">
-        <v>72</v>
-      </c>
-      <c r="M6" t="s">
-        <v>77</v>
-      </c>
-      <c r="O6" t="s">
-        <v>87</v>
-      </c>
-      <c r="P6" t="s">
-        <v>92</v>
-      </c>
-      <c r="R6" t="s">
-        <v>99</v>
       </c>
       <c r="W6" t="s">
         <v>111</v>
@@ -1833,34 +1831,34 @@
         <v>42</v>
       </c>
       <c r="C7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" t="s">
+        <v>78</v>
+      </c>
+      <c r="J7" t="s">
+        <v>148</v>
+      </c>
+      <c r="K7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L7" t="s">
+        <v>100</v>
+      </c>
+      <c r="M7" t="s">
         <v>158</v>
       </c>
-      <c r="D7" t="s">
-        <v>144</v>
-      </c>
-      <c r="G7" t="s">
-        <v>53</v>
-      </c>
-      <c r="H7" t="s">
-        <v>5</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="Q7" t="s">
         <v>66</v>
-      </c>
-      <c r="L7" t="s">
-        <v>133</v>
-      </c>
-      <c r="M7" t="s">
-        <v>78</v>
-      </c>
-      <c r="O7" t="s">
-        <v>148</v>
-      </c>
-      <c r="P7" t="s">
-        <v>93</v>
-      </c>
-      <c r="R7" t="s">
-        <v>100</v>
       </c>
       <c r="W7" s="2" t="s">
         <v>159</v>
@@ -1879,32 +1877,32 @@
       <c r="B8" t="s">
         <v>141</v>
       </c>
+      <c r="C8" t="s">
+        <v>153</v>
+      </c>
       <c r="D8" t="s">
-        <v>153</v>
+        <v>54</v>
+      </c>
+      <c r="E8" t="s">
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>145</v>
       </c>
       <c r="H8" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="J8" t="s">
+        <v>168</v>
+      </c>
+      <c r="K8" t="s">
+        <v>94</v>
+      </c>
+      <c r="L8" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q8" t="s">
         <v>6</v>
-      </c>
-      <c r="L8" t="s">
-        <v>145</v>
-      </c>
-      <c r="M8" t="s">
-        <v>79</v>
-      </c>
-      <c r="O8" t="s">
-        <v>168</v>
-      </c>
-      <c r="P8" t="s">
-        <v>94</v>
-      </c>
-      <c r="R8" t="s">
-        <v>101</v>
       </c>
       <c r="W8" t="s">
         <v>185</v>
@@ -1923,32 +1921,32 @@
       <c r="B9" t="s">
         <v>169</v>
       </c>
+      <c r="C9" t="s">
+        <v>162</v>
+      </c>
       <c r="D9" t="s">
-        <v>162</v>
+        <v>131</v>
+      </c>
+      <c r="E9" t="s">
+        <v>132</v>
       </c>
       <c r="G9" t="s">
-        <v>131</v>
+        <v>165</v>
       </c>
       <c r="H9" t="s">
-        <v>132</v>
+        <v>80</v>
       </c>
       <c r="J9" t="s">
+        <v>191</v>
+      </c>
+      <c r="K9" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q9" t="s">
         <v>149</v>
-      </c>
-      <c r="L9" t="s">
-        <v>165</v>
-      </c>
-      <c r="M9" t="s">
-        <v>80</v>
-      </c>
-      <c r="O9" t="s">
-        <v>191</v>
-      </c>
-      <c r="P9" t="s">
-        <v>89</v>
-      </c>
-      <c r="R9" t="s">
-        <v>102</v>
       </c>
       <c r="W9" t="s">
         <v>202</v>
@@ -1964,32 +1962,32 @@
       <c r="B10" t="s">
         <v>251</v>
       </c>
+      <c r="C10" t="s">
+        <v>201</v>
+      </c>
       <c r="D10" t="s">
-        <v>201</v>
+        <v>137</v>
+      </c>
+      <c r="E10" t="s">
+        <v>220</v>
       </c>
       <c r="G10" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="H10" t="s">
-        <v>220</v>
+        <v>135</v>
       </c>
       <c r="J10" t="s">
+        <v>233</v>
+      </c>
+      <c r="K10" t="s">
+        <v>95</v>
+      </c>
+      <c r="L10" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q10" t="s">
         <v>174</v>
-      </c>
-      <c r="L10" t="s">
-        <v>172</v>
-      </c>
-      <c r="M10" t="s">
-        <v>135</v>
-      </c>
-      <c r="O10" t="s">
-        <v>233</v>
-      </c>
-      <c r="P10" t="s">
-        <v>95</v>
-      </c>
-      <c r="R10" t="s">
-        <v>128</v>
       </c>
       <c r="W10" t="s">
         <v>260</v>
@@ -1999,106 +1997,106 @@
       <c r="A11" t="s">
         <v>130</v>
       </c>
+      <c r="C11" t="s">
+        <v>212</v>
+      </c>
       <c r="D11" t="s">
-        <v>212</v>
+        <v>139</v>
       </c>
       <c r="G11" t="s">
-        <v>139</v>
+        <v>175</v>
+      </c>
+      <c r="H11" t="s">
+        <v>166</v>
       </c>
       <c r="J11" t="s">
+        <v>243</v>
+      </c>
+      <c r="K11" t="s">
+        <v>140</v>
+      </c>
+      <c r="L11" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q11" t="s">
         <v>176</v>
-      </c>
-      <c r="L11" t="s">
-        <v>175</v>
-      </c>
-      <c r="M11" t="s">
-        <v>166</v>
-      </c>
-      <c r="O11" t="s">
-        <v>243</v>
-      </c>
-      <c r="P11" t="s">
-        <v>140</v>
-      </c>
-      <c r="R11" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>150</v>
       </c>
+      <c r="C12" t="s">
+        <v>227</v>
+      </c>
       <c r="D12" t="s">
-        <v>227</v>
+        <v>155</v>
       </c>
       <c r="G12" t="s">
-        <v>155</v>
+        <v>177</v>
+      </c>
+      <c r="H12" t="s">
+        <v>200</v>
       </c>
       <c r="J12" t="s">
+        <v>161</v>
+      </c>
+      <c r="K12" t="s">
+        <v>143</v>
+      </c>
+      <c r="L12" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q12" t="s">
         <v>179</v>
-      </c>
-      <c r="L12" t="s">
-        <v>177</v>
-      </c>
-      <c r="M12" t="s">
-        <v>200</v>
-      </c>
-      <c r="O12" t="s">
-        <v>161</v>
-      </c>
-      <c r="P12" t="s">
-        <v>143</v>
-      </c>
-      <c r="R12" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>156</v>
       </c>
+      <c r="C13" t="s">
+        <v>234</v>
+      </c>
       <c r="D13" t="s">
-        <v>234</v>
+        <v>157</v>
       </c>
       <c r="G13" t="s">
-        <v>157</v>
+        <v>180</v>
+      </c>
+      <c r="H13" t="s">
+        <v>257</v>
       </c>
       <c r="J13" t="s">
+        <v>81</v>
+      </c>
+      <c r="K13" t="s">
+        <v>142</v>
+      </c>
+      <c r="L13" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q13" t="s">
         <v>214</v>
-      </c>
-      <c r="L13" t="s">
-        <v>180</v>
-      </c>
-      <c r="M13" t="s">
-        <v>257</v>
-      </c>
-      <c r="O13" t="s">
-        <v>81</v>
-      </c>
-      <c r="P13" t="s">
-        <v>142</v>
-      </c>
-      <c r="R13" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>173</v>
       </c>
+      <c r="C14" t="s">
+        <v>262</v>
+      </c>
       <c r="D14" t="s">
-        <v>262</v>
+        <v>170</v>
       </c>
       <c r="G14" t="s">
-        <v>170</v>
+        <v>192</v>
+      </c>
+      <c r="K14" t="s">
+        <v>160</v>
       </c>
       <c r="L14" t="s">
-        <v>192</v>
-      </c>
-      <c r="P14" t="s">
-        <v>160</v>
-      </c>
-      <c r="R14" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2106,16 +2104,16 @@
       <c r="A15" t="s">
         <v>183</v>
       </c>
+      <c r="D15" t="s">
+        <v>190</v>
+      </c>
       <c r="G15" t="s">
-        <v>190</v>
+        <v>228</v>
+      </c>
+      <c r="K15" t="s">
+        <v>171</v>
       </c>
       <c r="L15" t="s">
-        <v>228</v>
-      </c>
-      <c r="P15" t="s">
-        <v>171</v>
-      </c>
-      <c r="R15" t="s">
         <v>182</v>
       </c>
     </row>
@@ -2123,16 +2121,16 @@
       <c r="A16" t="s">
         <v>197</v>
       </c>
+      <c r="D16" t="s">
+        <v>198</v>
+      </c>
       <c r="G16" t="s">
-        <v>198</v>
+        <v>236</v>
+      </c>
+      <c r="K16" t="s">
+        <v>181</v>
       </c>
       <c r="L16" t="s">
-        <v>236</v>
-      </c>
-      <c r="P16" t="s">
-        <v>181</v>
-      </c>
-      <c r="R16" t="s">
         <v>189</v>
       </c>
     </row>
@@ -2140,18 +2138,17 @@
       <c r="A17" t="s">
         <v>218</v>
       </c>
+      <c r="D17" t="s">
+        <v>199</v>
+      </c>
+      <c r="F17" s="3"/>
       <c r="G17" t="s">
-        <v>199</v>
-      </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3"/>
+        <v>239</v>
+      </c>
+      <c r="K17" t="s">
+        <v>208</v>
+      </c>
       <c r="L17" t="s">
-        <v>239</v>
-      </c>
-      <c r="P17" t="s">
-        <v>208</v>
-      </c>
-      <c r="R17" t="s">
         <v>206</v>
       </c>
     </row>
@@ -2159,30 +2156,36 @@
       <c r="A18" t="s">
         <v>230</v>
       </c>
+      <c r="D18" t="s">
+        <v>215</v>
+      </c>
       <c r="G18" t="s">
-        <v>215</v>
-      </c>
-      <c r="L18" t="s">
         <v>249</v>
       </c>
-      <c r="P18" t="s">
+      <c r="K18" t="s">
         <v>231</v>
       </c>
-      <c r="R18" s="4" t="s">
+      <c r="L18" s="4" t="s">
         <v>211</v>
       </c>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="4"/>
+      <c r="R18" s="4"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>241</v>
       </c>
-      <c r="G19" t="s">
+      <c r="D19" t="s">
         <v>226</v>
       </c>
-      <c r="P19" t="s">
+      <c r="K19" t="s">
         <v>248</v>
       </c>
-      <c r="R19" t="s">
+      <c r="L19" t="s">
         <v>219</v>
       </c>
     </row>
@@ -2190,13 +2193,13 @@
       <c r="A20" t="s">
         <v>250</v>
       </c>
-      <c r="G20" t="s">
+      <c r="D20" t="s">
         <v>246</v>
       </c>
-      <c r="P20" t="s">
+      <c r="K20" t="s">
         <v>252</v>
       </c>
-      <c r="R20" t="s">
+      <c r="L20" t="s">
         <v>225</v>
       </c>
     </row>
@@ -2204,26 +2207,26 @@
       <c r="A21" t="s">
         <v>184</v>
       </c>
-      <c r="G21" t="s">
+      <c r="D21" t="s">
         <v>247</v>
       </c>
-      <c r="P21" t="s">
+      <c r="K21" t="s">
         <v>258</v>
       </c>
-      <c r="R21" t="s">
+      <c r="L21" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="G22" t="s">
+      <c r="D22" t="s">
         <v>256</v>
       </c>
-      <c r="R22" t="s">
+      <c r="L22" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="R23" t="s">
+      <c r="L23" t="s">
         <v>253</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to mappings for ATS and ATP Comm Rate.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Lookup" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="274">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -654,9 +654,6 @@
     <t>Item</t>
   </si>
   <si>
-    <t>DK Ext Price</t>
-  </si>
-  <si>
     <t>Adj. Invoice Amount</t>
   </si>
   <si>
@@ -681,9 +678,6 @@
     <t>Top Mark</t>
   </si>
   <si>
-    <t>RES.EXT</t>
-  </si>
-  <si>
     <t>End Customer value</t>
   </si>
   <si>
@@ -844,6 +838,9 @@
   </si>
   <si>
     <t>GT Total</t>
+  </si>
+  <si>
+    <t>ATS Ext Price</t>
   </si>
 </sst>
 </file>
@@ -1265,7 +1262,7 @@
   <dimension ref="A1:AI2561"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="G13" sqref="G13:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2012,217 +2009,214 @@
         <v>210</v>
       </c>
       <c r="G12" t="s">
+        <v>273</v>
+      </c>
+      <c r="H12" t="s">
         <v>211</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>212</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>213</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>214</v>
       </c>
-      <c r="L12" t="s">
+      <c r="Q12" t="s">
         <v>215</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C13" t="s">
         <v>217</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>218</v>
       </c>
-      <c r="D13" t="s">
+      <c r="G13" t="s">
+        <v>227</v>
+      </c>
+      <c r="H13" t="s">
         <v>219</v>
       </c>
-      <c r="G13" t="s">
+      <c r="J13" t="s">
         <v>220</v>
       </c>
-      <c r="H13" t="s">
+      <c r="K13" t="s">
         <v>221</v>
       </c>
-      <c r="J13" t="s">
+      <c r="L13" t="s">
         <v>222</v>
       </c>
-      <c r="K13" t="s">
+      <c r="Q13" t="s">
         <v>223</v>
-      </c>
-      <c r="L13" t="s">
-        <v>224</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>224</v>
+      </c>
+      <c r="C14" t="s">
+        <v>225</v>
+      </c>
+      <c r="D14" t="s">
         <v>226</v>
       </c>
-      <c r="C14" t="s">
-        <v>227</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="G14" t="s">
+        <v>233</v>
+      </c>
+      <c r="H14" t="s">
         <v>228</v>
       </c>
-      <c r="G14" t="s">
+      <c r="K14" t="s">
         <v>229</v>
       </c>
-      <c r="H14" t="s">
+      <c r="L14" t="s">
         <v>230</v>
       </c>
-      <c r="K14" t="s">
-        <v>231</v>
-      </c>
-      <c r="L14" t="s">
-        <v>232</v>
-      </c>
       <c r="Q14" s="2" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D15" t="s">
+        <v>232</v>
+      </c>
+      <c r="G15" t="s">
+        <v>238</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="K15" t="s">
         <v>234</v>
       </c>
-      <c r="G15" t="s">
+      <c r="L15" t="s">
         <v>235</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="K15" t="s">
-        <v>236</v>
-      </c>
-      <c r="L15" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D16" t="s">
+        <v>237</v>
+      </c>
+      <c r="G16" t="s">
+        <v>243</v>
+      </c>
+      <c r="K16" t="s">
         <v>239</v>
       </c>
-      <c r="G16" t="s">
+      <c r="L16" t="s">
         <v>240</v>
-      </c>
-      <c r="K16" t="s">
-        <v>241</v>
-      </c>
-      <c r="L16" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D17" t="s">
+        <v>242</v>
+      </c>
+      <c r="G17" t="s">
+        <v>248</v>
+      </c>
+      <c r="K17" t="s">
         <v>244</v>
       </c>
-      <c r="G17" t="s">
+      <c r="L17" t="s">
         <v>245</v>
-      </c>
-      <c r="K17" t="s">
-        <v>246</v>
-      </c>
-      <c r="L17" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D18" t="s">
+        <v>247</v>
+      </c>
+      <c r="K18" t="s">
         <v>249</v>
       </c>
-      <c r="G18" t="s">
+      <c r="L18" t="s">
         <v>250</v>
-      </c>
-      <c r="K18" t="s">
-        <v>251</v>
-      </c>
-      <c r="L18" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>251</v>
+      </c>
+      <c r="D19" t="s">
+        <v>252</v>
+      </c>
+      <c r="K19" t="s">
         <v>253</v>
       </c>
-      <c r="D19" t="s">
+      <c r="L19" t="s">
         <v>254</v>
-      </c>
-      <c r="K19" t="s">
-        <v>255</v>
-      </c>
-      <c r="L19" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>255</v>
+      </c>
+      <c r="D20" t="s">
+        <v>256</v>
+      </c>
+      <c r="K20" t="s">
         <v>257</v>
       </c>
-      <c r="D20" t="s">
+      <c r="L20" t="s">
         <v>258</v>
-      </c>
-      <c r="K20" t="s">
-        <v>259</v>
-      </c>
-      <c r="L20" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>259</v>
+      </c>
+      <c r="D21" t="s">
+        <v>260</v>
+      </c>
+      <c r="K21" t="s">
         <v>261</v>
       </c>
-      <c r="D21" t="s">
+      <c r="L21" t="s">
         <v>262</v>
-      </c>
-      <c r="K21" t="s">
-        <v>263</v>
-      </c>
-      <c r="L21" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="K22" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L22" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L23" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="L24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4552,7 +4546,7 @@
     <row r="2349" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2350" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2350" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2351" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4767,7 +4761,7 @@
     <row r="2560" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2561" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2561" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Field Mappings updated. Finished ABR, working on rest.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="275">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -381,9 +381,6 @@
     <t>CommEarned</t>
   </si>
   <si>
-    <t>Sold To Name</t>
-  </si>
-  <si>
     <t>Purchase Ord. No.</t>
   </si>
   <si>
@@ -841,6 +838,12 @@
   </si>
   <si>
     <t>ATS Ext Price</t>
+  </si>
+  <si>
+    <t>Disti price [per pce]</t>
+  </si>
+  <si>
+    <t>Rep 1 rate</t>
   </si>
 </sst>
 </file>
@@ -1261,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2561"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1695,7 +1698,7 @@
         <v>115</v>
       </c>
       <c r="H5" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="I5" t="s">
         <v>117</v>
@@ -1710,513 +1713,516 @@
         <v>11</v>
       </c>
       <c r="M5" t="s">
+        <v>138</v>
+      </c>
+      <c r="N5" t="s">
         <v>120</v>
       </c>
-      <c r="N5" t="s">
+      <c r="P5" t="s">
         <v>121</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>122</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="U5" t="s">
         <v>123</v>
-      </c>
-      <c r="U5" t="s">
-        <v>124</v>
       </c>
       <c r="V5" t="s">
         <v>105</v>
       </c>
       <c r="W5" t="s">
+        <v>124</v>
+      </c>
+      <c r="X5" t="s">
         <v>125</v>
-      </c>
-      <c r="X5" t="s">
-        <v>126</v>
       </c>
       <c r="Y5" t="s">
         <v>24</v>
       </c>
       <c r="AB5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B6" t="s">
         <v>128</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>129</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>130</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>131</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>132</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>133</v>
       </c>
-      <c r="G6" t="s">
-        <v>134</v>
-      </c>
       <c r="H6" t="s">
+        <v>148</v>
+      </c>
+      <c r="J6" t="s">
         <v>135</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>136</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>137</v>
       </c>
-      <c r="L6" t="s">
-        <v>138</v>
-      </c>
       <c r="M6" t="s">
+        <v>152</v>
+      </c>
+      <c r="P6" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q6" t="s">
         <v>139</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="W6" t="s">
         <v>140</v>
       </c>
-      <c r="W6" t="s">
+      <c r="X6" t="s">
         <v>141</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>142</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" t="s">
         <v>144</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>145</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>146</v>
-      </c>
-      <c r="D7" t="s">
-        <v>147</v>
       </c>
       <c r="E7" t="s">
         <v>4</v>
       </c>
+      <c r="F7" t="s">
+        <v>163</v>
+      </c>
       <c r="G7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H7" t="s">
+        <v>177</v>
+      </c>
+      <c r="J7" t="s">
         <v>149</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>150</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>151</v>
       </c>
-      <c r="L7" t="s">
-        <v>152</v>
-      </c>
       <c r="M7" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q7" t="s">
         <v>153</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="W7" t="s">
         <v>154</v>
       </c>
-      <c r="W7" t="s">
+      <c r="X7" t="s">
         <v>155</v>
       </c>
-      <c r="X7" t="s">
+      <c r="Y7" t="s">
         <v>156</v>
-      </c>
-      <c r="Y7" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" t="s">
         <v>158</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>159</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>160</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>161</v>
       </c>
-      <c r="E8" t="s">
+      <c r="G8" t="s">
         <v>162</v>
       </c>
-      <c r="G8" t="s">
-        <v>163</v>
-      </c>
       <c r="H8" t="s">
+        <v>190</v>
+      </c>
+      <c r="J8" t="s">
         <v>164</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>165</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>166</v>
-      </c>
-      <c r="L8" t="s">
-        <v>167</v>
-      </c>
-      <c r="M8" t="s">
-        <v>168</v>
       </c>
       <c r="Q8" t="s">
         <v>16</v>
       </c>
       <c r="W8" t="s">
+        <v>168</v>
+      </c>
+      <c r="X8" t="s">
         <v>169</v>
       </c>
-      <c r="X8" t="s">
+      <c r="Y8" t="s">
         <v>170</v>
-      </c>
-      <c r="Y8" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B9" t="s">
         <v>172</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>173</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>174</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>175</v>
       </c>
-      <c r="E9" t="s">
+      <c r="G9" t="s">
         <v>176</v>
       </c>
-      <c r="G9" t="s">
-        <v>177</v>
-      </c>
       <c r="H9" t="s">
+        <v>202</v>
+      </c>
+      <c r="J9" t="s">
         <v>178</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>179</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>180</v>
       </c>
-      <c r="L9" t="s">
+      <c r="Q9" t="s">
         <v>181</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="W9" t="s">
         <v>182</v>
       </c>
-      <c r="W9" t="s">
+      <c r="X9" t="s">
         <v>183</v>
-      </c>
-      <c r="X9" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="10" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>184</v>
+      </c>
+      <c r="B10" t="s">
         <v>185</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>186</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>187</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>188</v>
       </c>
-      <c r="E10" t="s">
+      <c r="G10" t="s">
         <v>189</v>
       </c>
-      <c r="G10" t="s">
-        <v>190</v>
-      </c>
       <c r="H10" t="s">
+        <v>210</v>
+      </c>
+      <c r="J10" t="s">
         <v>191</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>192</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>193</v>
       </c>
-      <c r="L10" t="s">
+      <c r="Q10" t="s">
         <v>194</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="W10" t="s">
         <v>195</v>
       </c>
-      <c r="W10" t="s">
+      <c r="Y10" t="s">
         <v>196</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="11" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" t="s">
         <v>198</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>199</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>200</v>
       </c>
-      <c r="D11" t="s">
+      <c r="G11" t="s">
         <v>201</v>
       </c>
-      <c r="G11" t="s">
-        <v>202</v>
-      </c>
       <c r="H11" t="s">
+        <v>218</v>
+      </c>
+      <c r="J11" t="s">
         <v>203</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>204</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>205</v>
       </c>
-      <c r="L11" t="s">
+      <c r="Q11" t="s">
         <v>206</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="12" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>207</v>
+      </c>
+      <c r="C12" t="s">
         <v>208</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>209</v>
       </c>
-      <c r="D12" t="s">
-        <v>210</v>
-      </c>
       <c r="G12" t="s">
-        <v>273</v>
-      </c>
-      <c r="H12" t="s">
+        <v>272</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="J12" t="s">
         <v>211</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>212</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>213</v>
       </c>
-      <c r="L12" t="s">
+      <c r="Q12" t="s">
         <v>214</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>215</v>
+      </c>
+      <c r="C13" t="s">
         <v>216</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>217</v>
       </c>
-      <c r="D13" t="s">
-        <v>218</v>
-      </c>
       <c r="G13" t="s">
-        <v>227</v>
-      </c>
-      <c r="H13" t="s">
+        <v>226</v>
+      </c>
+      <c r="J13" t="s">
         <v>219</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>220</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>221</v>
       </c>
-      <c r="L13" t="s">
+      <c r="Q13" t="s">
         <v>222</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
+        <v>223</v>
+      </c>
+      <c r="C14" t="s">
         <v>224</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>225</v>
       </c>
-      <c r="D14" t="s">
-        <v>226</v>
-      </c>
       <c r="G14" t="s">
-        <v>233</v>
-      </c>
-      <c r="H14" t="s">
+        <v>232</v>
+      </c>
+      <c r="J14" t="s">
+        <v>274</v>
+      </c>
+      <c r="K14" t="s">
         <v>228</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>229</v>
       </c>
-      <c r="L14" t="s">
-        <v>230</v>
-      </c>
       <c r="Q14" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D15" t="s">
         <v>231</v>
       </c>
-      <c r="D15" t="s">
-        <v>232</v>
-      </c>
       <c r="G15" t="s">
-        <v>238</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
       <c r="K15" t="s">
+        <v>233</v>
+      </c>
+      <c r="L15" t="s">
         <v>234</v>
-      </c>
-      <c r="L15" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="16" spans="1:35" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>235</v>
+      </c>
+      <c r="D16" t="s">
         <v>236</v>
       </c>
-      <c r="D16" t="s">
-        <v>237</v>
-      </c>
       <c r="G16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="K16" t="s">
+        <v>238</v>
+      </c>
+      <c r="L16" t="s">
         <v>239</v>
-      </c>
-      <c r="L16" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>240</v>
+      </c>
+      <c r="D17" t="s">
         <v>241</v>
       </c>
-      <c r="D17" t="s">
-        <v>242</v>
-      </c>
       <c r="G17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K17" t="s">
+        <v>243</v>
+      </c>
+      <c r="L17" t="s">
         <v>244</v>
-      </c>
-      <c r="L17" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>245</v>
+      </c>
+      <c r="D18" t="s">
         <v>246</v>
       </c>
-      <c r="D18" t="s">
-        <v>247</v>
+      <c r="G18" t="s">
+        <v>116</v>
       </c>
       <c r="K18" t="s">
+        <v>248</v>
+      </c>
+      <c r="L18" t="s">
         <v>249</v>
-      </c>
-      <c r="L18" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>250</v>
+      </c>
+      <c r="D19" t="s">
         <v>251</v>
       </c>
-      <c r="D19" t="s">
+      <c r="G19" t="s">
+        <v>227</v>
+      </c>
+      <c r="K19" t="s">
         <v>252</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>253</v>
-      </c>
-      <c r="L19" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>254</v>
+      </c>
+      <c r="D20" t="s">
         <v>255</v>
       </c>
-      <c r="D20" t="s">
+      <c r="K20" t="s">
         <v>256</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>257</v>
-      </c>
-      <c r="L20" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>258</v>
+      </c>
+      <c r="D21" t="s">
         <v>259</v>
       </c>
-      <c r="D21" t="s">
+      <c r="K21" t="s">
         <v>260</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>261</v>
-      </c>
-      <c r="L21" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D22" t="s">
+        <v>262</v>
+      </c>
+      <c r="K22" t="s">
+        <v>247</v>
+      </c>
+      <c r="L22" t="s">
         <v>263</v>
-      </c>
-      <c r="K22" t="s">
-        <v>248</v>
-      </c>
-      <c r="L22" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
+        <v>264</v>
+      </c>
+      <c r="L23" t="s">
         <v>265</v>
-      </c>
-      <c r="L23" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L24" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4546,7 +4552,7 @@
     <row r="2349" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2350" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2350" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="2351" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4761,7 +4767,7 @@
     <row r="2560" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2561" spans="1:1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2561" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished updating Paid-On Revenue mappings.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -1264,8 +1264,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2561"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1819,7 +1819,7 @@
         <v>147</v>
       </c>
       <c r="H7" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="J7" t="s">
         <v>149</v>
@@ -1866,7 +1866,7 @@
         <v>162</v>
       </c>
       <c r="H8" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="J8" t="s">
         <v>164</v>
@@ -1910,7 +1910,7 @@
         <v>176</v>
       </c>
       <c r="H9" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="J9" t="s">
         <v>178</v>
@@ -1951,7 +1951,7 @@
         <v>189</v>
       </c>
       <c r="H10" t="s">
-        <v>210</v>
+        <v>218</v>
       </c>
       <c r="J10" t="s">
         <v>191</v>
@@ -1988,8 +1988,8 @@
       <c r="G11" t="s">
         <v>201</v>
       </c>
-      <c r="H11" t="s">
-        <v>218</v>
+      <c r="H11" s="2" t="s">
+        <v>271</v>
       </c>
       <c r="J11" t="s">
         <v>203</v>
@@ -2017,9 +2017,6 @@
       <c r="G12" t="s">
         <v>272</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="J12" t="s">
         <v>211</v>
       </c>
@@ -2176,6 +2173,9 @@
       </c>
       <c r="D20" t="s">
         <v>255</v>
+      </c>
+      <c r="G20" t="s">
+        <v>177</v>
       </c>
       <c r="K20" t="s">
         <v>256</v>

</xml_diff>

<commit_message>
Made ATS sheet names more flexible.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="276">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -844,6 +844,9 @@
   </si>
   <si>
     <t>Rep 1 rate</t>
+  </si>
+  <si>
+    <t>DATE</t>
   </si>
 </sst>
 </file>
@@ -1264,8 +1267,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2561"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:H11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2225,7 +2228,11 @@
         <v>266</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L25" t="s">
+        <v>275</v>
+      </c>
+    </row>
     <row r="26" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fixed issues with GLO file.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="277">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -847,6 +847,9 @@
   </si>
   <si>
     <t>DATE</t>
+  </si>
+  <si>
+    <t>Com</t>
   </si>
 </sst>
 </file>
@@ -1267,8 +1270,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2561"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2215,6 +2218,9 @@
     <row r="23" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D23" t="s">
         <v>264</v>
+      </c>
+      <c r="K23" t="s">
+        <v>276</v>
       </c>
       <c r="L23" t="s">
         <v>265</v>

</xml_diff>

<commit_message>
Added the Uknowns to Lookup Master and worked it into the code.
</commit_message>
<xml_diff>
--- a/fieldMappings.xlsx
+++ b/fieldMappings.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="278">
   <si>
     <t>Reported Customer</t>
   </si>
@@ -850,6 +850,9 @@
   </si>
   <si>
     <t>Com</t>
+  </si>
+  <si>
+    <t>Sold To Name</t>
   </si>
 </sst>
 </file>
@@ -867,6 +870,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1270,8 +1274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI2561"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1882,6 +1886,9 @@
       </c>
       <c r="L8" t="s">
         <v>166</v>
+      </c>
+      <c r="M8" t="s">
+        <v>277</v>
       </c>
       <c r="Q8" t="s">
         <v>16</v>

</xml_diff>